<commit_message>
PLEASE DON'T COMMIT THE ENV FILE
</commit_message>
<xml_diff>
--- a/The Plan.xlsx
+++ b/The Plan.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shark\OneDrive\Assesments\Software Engineering\VaultPad\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18355CB3-8027-4A4B-AB26-55D99956A6B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5FDA46-ED19-4898-81C6-C5821452DC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{431A7C84-B193-4DE8-B354-2F03DB034E92}"/>
   </bookViews>
@@ -280,32 +280,32 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E415910F-E1C5-4B14-9438-A71FE35E7CA4}">
   <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" zoomScale="66" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -747,9 +747,9 @@
         <v>26</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
       <c r="G4" s="2"/>
       <c r="H4" s="2"/>
       <c r="I4" s="2"/>
@@ -765,7 +765,7 @@
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="2"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
@@ -800,8 +800,8 @@
         <v>27</v>
       </c>
       <c r="C7" s="6"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
       <c r="F7" s="2"/>
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
@@ -1101,32 +1101,32 @@
         <v>29</v>
       </c>
       <c r="B24" s="15"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="10"/>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
+      <c r="C24" s="14"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="18"/>
+      <c r="F24" s="18"/>
+      <c r="G24" s="18"/>
+      <c r="H24" s="18"/>
+      <c r="I24" s="18"/>
+      <c r="J24" s="18"/>
+      <c r="K24" s="18"/>
+      <c r="L24" s="18"/>
+      <c r="M24" s="18"/>
     </row>
     <row r="25" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="15"/>
       <c r="B25" s="15"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="10"/>
-      <c r="F25" s="10"/>
-      <c r="G25" s="10"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="10"/>
-      <c r="J25" s="10"/>
-      <c r="K25" s="10"/>
-      <c r="L25" s="10"/>
-      <c r="M25" s="10"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="18"/>
+      <c r="E25" s="18"/>
+      <c r="F25" s="18"/>
+      <c r="G25" s="18"/>
+      <c r="H25" s="18"/>
+      <c r="I25" s="18"/>
+      <c r="J25" s="18"/>
+      <c r="K25" s="18"/>
+      <c r="L25" s="18"/>
+      <c r="M25" s="18"/>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
@@ -1146,7 +1146,7 @@
       <c r="M26" s="2"/>
     </row>
     <row r="27" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="12" t="s">
+      <c r="A27" s="16" t="s">
         <v>32</v>
       </c>
       <c r="B27" s="3" t="s">
@@ -1165,7 +1165,7 @@
       <c r="M27" s="2"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="12"/>
+      <c r="A28" s="16"/>
       <c r="B28" s="3" t="s">
         <v>27</v>
       </c>
@@ -1182,7 +1182,7 @@
       <c r="M28" s="2"/>
     </row>
     <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="12" t="s">
+      <c r="A29" s="16" t="s">
         <v>33</v>
       </c>
       <c r="B29" s="3" t="s">
@@ -1201,7 +1201,7 @@
       <c r="M29" s="2"/>
     </row>
     <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="12"/>
+      <c r="A30" s="16"/>
       <c r="B30" s="3" t="s">
         <v>27</v>
       </c>
@@ -1217,7 +1217,7 @@
       <c r="M30" s="2"/>
     </row>
     <row r="31" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="12" t="s">
+      <c r="A31" s="16" t="s">
         <v>34</v>
       </c>
       <c r="B31" s="3" t="s">
@@ -1236,7 +1236,7 @@
       <c r="M31" s="2"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A32" s="12"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="3" t="s">
         <v>27</v>
       </c>
@@ -1253,7 +1253,7 @@
       <c r="M32" s="2"/>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A33" s="12" t="s">
+      <c r="A33" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B33" s="3" t="s">
@@ -1272,7 +1272,7 @@
       <c r="M33" s="2"/>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="12"/>
+      <c r="A34" s="16"/>
       <c r="B34" s="3" t="s">
         <v>27</v>
       </c>
@@ -1289,7 +1289,7 @@
       <c r="M34" s="2"/>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A35" s="12" t="s">
+      <c r="A35" s="16" t="s">
         <v>29</v>
       </c>
       <c r="B35" s="3"/>
@@ -1306,7 +1306,7 @@
       <c r="M35" s="2"/>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="16"/>
       <c r="B36" s="3"/>
       <c r="C36" s="6"/>
       <c r="D36" s="2"/>
@@ -1338,7 +1338,7 @@
       <c r="M37" s="2"/>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="17" t="s">
         <v>31</v>
       </c>
       <c r="B38" s="5" t="s">
@@ -1357,7 +1357,7 @@
       <c r="M38" s="2"/>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
+      <c r="A39" s="17"/>
       <c r="B39" s="5" t="s">
         <v>27</v>
       </c>
@@ -1374,7 +1374,7 @@
       <c r="M39" s="2"/>
     </row>
     <row r="40" spans="1:13" ht="14.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B40" s="5" t="s">
@@ -1393,7 +1393,7 @@
       <c r="M40" s="2"/>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
+      <c r="A41" s="17"/>
       <c r="B41" s="5" t="s">
         <v>27</v>
       </c>
@@ -1410,7 +1410,7 @@
       <c r="M41" s="2"/>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="17" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -1429,7 +1429,7 @@
       <c r="M42" s="2"/>
     </row>
     <row r="43" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
+      <c r="A43" s="17"/>
       <c r="B43" s="5" t="s">
         <v>27</v>
       </c>
@@ -1446,29 +1446,29 @@
       <c r="M43" s="2"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="B44" s="16"/>
+      <c r="B44" s="11"/>
       <c r="C44" s="7"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A45" s="13"/>
-      <c r="B45" s="16"/>
+      <c r="A45" s="17"/>
+      <c r="B45" s="11"/>
       <c r="C45" s="7"/>
     </row>
     <row r="46" spans="1:13" ht="29" x14ac:dyDescent="0.35">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="B46" s="14"/>
+      <c r="B46" s="10"/>
       <c r="C46" s="7"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A47" s="18" t="s">
+      <c r="A47" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C47" s="6"/>
@@ -1484,8 +1484,8 @@
       <c r="M47" s="2"/>
     </row>
     <row r="48" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A48" s="18"/>
-      <c r="B48" s="14" t="s">
+      <c r="A48" s="13"/>
+      <c r="B48" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C48" s="6"/>
@@ -1501,58 +1501,78 @@
       <c r="M48" s="2"/>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A49" s="18" t="s">
+      <c r="A49" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C49" s="7"/>
       <c r="L49" s="9"/>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A50" s="18"/>
-      <c r="B50" s="14" t="s">
+      <c r="A50" s="13"/>
+      <c r="B50" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C50" s="7"/>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A51" s="18" t="s">
+      <c r="A51" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C51" s="7"/>
       <c r="L51" s="9"/>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A52" s="18"/>
-      <c r="B52" s="14" t="s">
+      <c r="A52" s="13"/>
+      <c r="B52" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C52" s="7"/>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A53" s="18" t="s">
+      <c r="A53" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="10" t="s">
         <v>26</v>
       </c>
       <c r="C53" s="7"/>
       <c r="L53" s="9"/>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A54" s="18"/>
-      <c r="B54" s="14" t="s">
+      <c r="A54" s="13"/>
+      <c r="B54" s="10" t="s">
         <v>27</v>
       </c>
       <c r="C54" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="36">
+    <mergeCell ref="J24:J25"/>
+    <mergeCell ref="K24:K25"/>
+    <mergeCell ref="L24:L25"/>
+    <mergeCell ref="M24:M25"/>
+    <mergeCell ref="D24:D25"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="F24:F25"/>
+    <mergeCell ref="G24:G25"/>
+    <mergeCell ref="H24:H25"/>
+    <mergeCell ref="I24:I25"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="A47:A48"/>
     <mergeCell ref="A49:A50"/>
     <mergeCell ref="A51:A52"/>
@@ -1569,26 +1589,6 @@
     <mergeCell ref="A38:A39"/>
     <mergeCell ref="A42:A43"/>
     <mergeCell ref="A44:A45"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="J24:J25"/>
-    <mergeCell ref="K24:K25"/>
-    <mergeCell ref="L24:L25"/>
-    <mergeCell ref="M24:M25"/>
-    <mergeCell ref="D24:D25"/>
-    <mergeCell ref="E24:E25"/>
-    <mergeCell ref="F24:F25"/>
-    <mergeCell ref="G24:G25"/>
-    <mergeCell ref="H24:H25"/>
-    <mergeCell ref="I24:I25"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>